<commit_message>
DataValidation.xlsx updated. It had 42 rules at sheet 2, now it has 16.
</commit_message>
<xml_diff>
--- a/ClosedXML_Tests/Resource/Examples/Misc/DataValidation.xlsx
+++ b/ClosedXML_Tests/Resource/Examples/Misc/DataValidation.xlsx
@@ -420,21 +420,13 @@
     </x:row>
   </x:sheetData>
   <x:dataValidations count="7">
+    <x:dataValidation type="decimal" errorStyle="stop" operator="between" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="A1:A1">
+      <x:formula1>1</x:formula1>
+      <x:formula2>5</x:formula2>
+    </x:dataValidation>
     <x:dataValidation type="whole" errorStyle="warning" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Number out of range" error="This cell only allows the number 2." promptTitle="" prompt="" sqref="A2:A3">
       <x:formula1>2</x:formula1>
       <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="whole" errorStyle="stop" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="B1:B2">
-      <x:formula1>1</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="whole" errorStyle="stop" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="B3:B4">
-      <x:formula1>2</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="between" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="A1:A1">
-      <x:formula1>1</x:formula1>
-      <x:formula2>5</x:formula2>
     </x:dataValidation>
     <x:dataValidation type="date" errorStyle="stop" operator="greaterThanOrEqual" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="Can't party like it's 1999." prompt="Please enter a date in this century." sqref="A4:A4">
       <x:formula1>36526</x:formula1>
@@ -446,6 +438,14 @@
     </x:dataValidation>
     <x:dataValidation type="list" errorStyle="stop" operator="between" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="A6:A6">
       <x:formula1>=YesNo</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="whole" errorStyle="stop" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="B1:B2">
+      <x:formula1>1</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="whole" errorStyle="stop" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="B3:B4">
+      <x:formula1>2</x:formula1>
       <x:formula2/>
     </x:dataValidation>
   </x:dataValidations>
@@ -468,7 +468,7 @@
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15"/>
   <x:cols>
-    <x:col min="1" max="7" width="9.140625" style="0" customWidth="1"/>
+    <x:col min="1" max="4" width="9.140625" style="0" customWidth="1"/>
   </x:cols>
   <x:sheetData>
     <x:row r="1" spans="1:7">
@@ -532,173 +532,69 @@
       <x:c r="E14" s="1" t="s"/>
     </x:row>
   </x:sheetData>
-  <x:dataValidations count="42">
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="B3:B3">
+  <x:dataValidations count="16">
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="A1:A2">
+      <x:formula1>1</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="B1:B1">
+      <x:formula1>1</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="C4:C7">
+      <x:formula1>1</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="D4:D4">
+      <x:formula1>1</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="D7:D7">
+      <x:formula1>1</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="F4:F5">
+      <x:formula1>1</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="A11:A14">
+      <x:formula1>2</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="B13:B14">
+      <x:formula1>2</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="E11:E14">
+      <x:formula1>2</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="C11:C12">
+      <x:formula1>2</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="D13:D14">
+      <x:formula1>2</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="B2:B12">
       <x:formula1>3</x:formula1>
       <x:formula2/>
     </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="B8:B10">
-      <x:formula1>3</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="A1:A1">
-      <x:formula1>1</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="B1:B1">
-      <x:formula1>1</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="A2:A2">
-      <x:formula1>1</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="B2:B2">
-      <x:formula1>3</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="B4:B4">
-      <x:formula1>3</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="C4:C4">
-      <x:formula1>1</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="D4:D4">
-      <x:formula1>1</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="F4:F4">
-      <x:formula1>1</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="G4:G4">
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="D5:D6">
+      <x:formula1>4</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="C13:C14">
       <x:formula1>5</x:formula1>
       <x:formula2/>
     </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="B5:B5">
-      <x:formula1>3</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="C5:C5">
-      <x:formula1>1</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="D5:D5">
-      <x:formula1>4</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="F5:F5">
-      <x:formula1>1</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="G5:G5">
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="D11:D12">
       <x:formula1>5</x:formula1>
       <x:formula2/>
     </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="B6:B6">
-      <x:formula1>3</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="C6:C6">
-      <x:formula1>1</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="D6:D6">
-      <x:formula1>4</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="B7:B7">
-      <x:formula1>3</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="C7:C7">
-      <x:formula1>1</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="D7:D7">
-      <x:formula1>1</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="A11:A11">
-      <x:formula1>2</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="B11:B11">
-      <x:formula1>3</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="C11:C11">
-      <x:formula1>2</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="D11:D11">
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="G4:G5">
       <x:formula1>5</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="E11:E11">
-      <x:formula1>2</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="A12:A12">
-      <x:formula1>2</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="B12:B12">
-      <x:formula1>3</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="C12:C12">
-      <x:formula1>2</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="D12:D12">
-      <x:formula1>5</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="E12:E12">
-      <x:formula1>2</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="A13:A13">
-      <x:formula1>2</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="B13:B13">
-      <x:formula1>2</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="C13:C13">
-      <x:formula1>5</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="D13:D13">
-      <x:formula1>2</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="E13:E13">
-      <x:formula1>2</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="A14:A14">
-      <x:formula1>2</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="B14:B14">
-      <x:formula1>2</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="C14:C14">
-      <x:formula1>5</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="D14:D14">
-      <x:formula1>2</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="E14:E14">
-      <x:formula1>2</x:formula1>
       <x:formula2/>
     </x:dataValidation>
   </x:dataValidations>

</xml_diff>

<commit_message>
Fix issues with data validation rules (#718)
* Failing tests added

* Modified logic of cell DataValidation rules

* DataValidation.xlsx updated. It had 42 rules at sheet 2, now it has 16.

* Tests muted until formula shifting fixed

* Reading DataValidation rules for ranges made pure

* Restore DataValidation implicit creation to avoid breaking changes. Fix clearing data validation.

* Original test restored (use DataValidation instead of SetDataValidation)
</commit_message>
<xml_diff>
--- a/ClosedXML_Tests/Resource/Examples/Misc/DataValidation.xlsx
+++ b/ClosedXML_Tests/Resource/Examples/Misc/DataValidation.xlsx
@@ -420,21 +420,13 @@
     </x:row>
   </x:sheetData>
   <x:dataValidations count="7">
+    <x:dataValidation type="decimal" errorStyle="stop" operator="between" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="A1:A1">
+      <x:formula1>1</x:formula1>
+      <x:formula2>5</x:formula2>
+    </x:dataValidation>
     <x:dataValidation type="whole" errorStyle="warning" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Number out of range" error="This cell only allows the number 2." promptTitle="" prompt="" sqref="A2:A3">
       <x:formula1>2</x:formula1>
       <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="whole" errorStyle="stop" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="B1:B2">
-      <x:formula1>1</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="whole" errorStyle="stop" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="B3:B4">
-      <x:formula1>2</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="between" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="A1:A1">
-      <x:formula1>1</x:formula1>
-      <x:formula2>5</x:formula2>
     </x:dataValidation>
     <x:dataValidation type="date" errorStyle="stop" operator="greaterThanOrEqual" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="Can't party like it's 1999." prompt="Please enter a date in this century." sqref="A4:A4">
       <x:formula1>36526</x:formula1>
@@ -446,6 +438,14 @@
     </x:dataValidation>
     <x:dataValidation type="list" errorStyle="stop" operator="between" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="A6:A6">
       <x:formula1>=YesNo</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="whole" errorStyle="stop" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="B1:B2">
+      <x:formula1>1</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="whole" errorStyle="stop" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="B3:B4">
+      <x:formula1>2</x:formula1>
       <x:formula2/>
     </x:dataValidation>
   </x:dataValidations>
@@ -468,7 +468,7 @@
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15"/>
   <x:cols>
-    <x:col min="1" max="7" width="9.140625" style="0" customWidth="1"/>
+    <x:col min="1" max="4" width="9.140625" style="0" customWidth="1"/>
   </x:cols>
   <x:sheetData>
     <x:row r="1" spans="1:7">
@@ -532,173 +532,69 @@
       <x:c r="E14" s="1" t="s"/>
     </x:row>
   </x:sheetData>
-  <x:dataValidations count="42">
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="B3:B3">
+  <x:dataValidations count="16">
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="A1:A2">
+      <x:formula1>1</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="B1:B1">
+      <x:formula1>1</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="C4:C7">
+      <x:formula1>1</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="D4:D4">
+      <x:formula1>1</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="D7:D7">
+      <x:formula1>1</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="F4:F5">
+      <x:formula1>1</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="A11:A14">
+      <x:formula1>2</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="B13:B14">
+      <x:formula1>2</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="E11:E14">
+      <x:formula1>2</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="C11:C12">
+      <x:formula1>2</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="D13:D14">
+      <x:formula1>2</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="B2:B12">
       <x:formula1>3</x:formula1>
       <x:formula2/>
     </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="B8:B10">
-      <x:formula1>3</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="A1:A1">
-      <x:formula1>1</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="B1:B1">
-      <x:formula1>1</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="A2:A2">
-      <x:formula1>1</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="B2:B2">
-      <x:formula1>3</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="B4:B4">
-      <x:formula1>3</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="C4:C4">
-      <x:formula1>1</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="D4:D4">
-      <x:formula1>1</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="F4:F4">
-      <x:formula1>1</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="G4:G4">
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="D5:D6">
+      <x:formula1>4</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="C13:C14">
       <x:formula1>5</x:formula1>
       <x:formula2/>
     </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="B5:B5">
-      <x:formula1>3</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="C5:C5">
-      <x:formula1>1</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="D5:D5">
-      <x:formula1>4</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="F5:F5">
-      <x:formula1>1</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="G5:G5">
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="D11:D12">
       <x:formula1>5</x:formula1>
       <x:formula2/>
     </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="B6:B6">
-      <x:formula1>3</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="C6:C6">
-      <x:formula1>1</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="D6:D6">
-      <x:formula1>4</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="B7:B7">
-      <x:formula1>3</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="C7:C7">
-      <x:formula1>1</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="D7:D7">
-      <x:formula1>1</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="A11:A11">
-      <x:formula1>2</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="B11:B11">
-      <x:formula1>3</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="C11:C11">
-      <x:formula1>2</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="D11:D11">
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="G4:G5">
       <x:formula1>5</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="E11:E11">
-      <x:formula1>2</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="A12:A12">
-      <x:formula1>2</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="B12:B12">
-      <x:formula1>3</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="C12:C12">
-      <x:formula1>2</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="D12:D12">
-      <x:formula1>5</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="E12:E12">
-      <x:formula1>2</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="A13:A13">
-      <x:formula1>2</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="B13:B13">
-      <x:formula1>2</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="C13:C13">
-      <x:formula1>5</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="D13:D13">
-      <x:formula1>2</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="E13:E13">
-      <x:formula1>2</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="A14:A14">
-      <x:formula1>2</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="B14:B14">
-      <x:formula1>2</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="C14:C14">
-      <x:formula1>5</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="D14:D14">
-      <x:formula1>2</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="E14:E14">
-      <x:formula1>2</x:formula1>
       <x:formula2/>
     </x:dataValidation>
   </x:dataValidations>

</xml_diff>

<commit_message>
Data validaton rules consolidation implemented
</commit_message>
<xml_diff>
--- a/ClosedXML_Tests/Resource/Examples/Misc/DataValidation.xlsx
+++ b/ClosedXML_Tests/Resource/Examples/Misc/DataValidation.xlsx
@@ -532,48 +532,12 @@
       <x:c r="E14" s="1" t="s"/>
     </x:row>
   </x:sheetData>
-  <x:dataValidations count="16">
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="A1:A2">
+  <x:dataValidations count="5">
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="A1:B1 A2:A2 C4:D4 F4:F5 C5:C7 D7:D7">
       <x:formula1>1</x:formula1>
       <x:formula2/>
     </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="B1:B1">
-      <x:formula1>1</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="C4:C7">
-      <x:formula1>1</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="D4:D4">
-      <x:formula1>1</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="D7:D7">
-      <x:formula1>1</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="F4:F5">
-      <x:formula1>1</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="A11:A14">
-      <x:formula1>2</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="B13:B14">
-      <x:formula1>2</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="E11:E14">
-      <x:formula1>2</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="C11:C12">
-      <x:formula1>2</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="D13:D14">
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="A11:A14 C11:C12 E11:E14 B13:B14 D13:D14">
       <x:formula1>2</x:formula1>
       <x:formula2/>
     </x:dataValidation>
@@ -585,15 +549,7 @@
       <x:formula1>4</x:formula1>
       <x:formula2/>
     </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="C13:C14">
-      <x:formula1>5</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="D11:D12">
-      <x:formula1>5</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="G4:G5">
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="G4:G5 D11:D12 C13:C14">
       <x:formula1>5</x:formula1>
       <x:formula2/>
     </x:dataValidation>
@@ -761,48 +717,12 @@
       <x:c r="E14" s="1" t="s"/>
     </x:row>
   </x:sheetData>
-  <x:dataValidations count="16">
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="A1:A2">
+  <x:dataValidations count="5">
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="A1:B1 A2:A2 C4:D4 F4:F5 C5:C7 D7:D7">
       <x:formula1>1</x:formula1>
       <x:formula2/>
     </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="B1:B1">
-      <x:formula1>1</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="C4:C7">
-      <x:formula1>1</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="D4:D4">
-      <x:formula1>1</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="D7:D7">
-      <x:formula1>1</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="F4:F5">
-      <x:formula1>1</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="A11:A14">
-      <x:formula1>2</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="B13:B14">
-      <x:formula1>2</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="E11:E14">
-      <x:formula1>2</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="C11:C12">
-      <x:formula1>2</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="D13:D14">
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="A11:A14 C11:C12 E11:E14 B13:B14 D13:D14">
       <x:formula1>2</x:formula1>
       <x:formula2/>
     </x:dataValidation>
@@ -814,15 +734,7 @@
       <x:formula1>4</x:formula1>
       <x:formula2/>
     </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="C13:C14">
-      <x:formula1>5</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="D11:D12">
-      <x:formula1>5</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="G4:G5">
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="G4:G5 D11:D12 C13:C14">
       <x:formula1>5</x:formula1>
       <x:formula2/>
     </x:dataValidation>
@@ -972,164 +884,24 @@
       <x:c r="E14" s="1" t="s"/>
     </x:row>
   </x:sheetData>
-  <x:dataValidations count="40">
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="A1:A1">
+  <x:dataValidations count="5">
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="A1:B1 A2:A2 C4:D4 F4:F5 C5:C7 D7:D7">
       <x:formula1>1</x:formula1>
       <x:formula2/>
     </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="B1:B1">
-      <x:formula1>1</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="A2:A2">
-      <x:formula1>1</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="B2:B2">
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="B2:B12">
       <x:formula1>3</x:formula1>
       <x:formula2/>
     </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="B4:B4">
-      <x:formula1>3</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="C4:C4">
-      <x:formula1>1</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="D4:D4">
-      <x:formula1>1</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="F4:F4">
-      <x:formula1>1</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="G4:G4">
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="G4:G5 D11:D12 C13:C14">
       <x:formula1>5</x:formula1>
       <x:formula2/>
     </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="B5:B5">
-      <x:formula1>3</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="C5:C5">
-      <x:formula1>1</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="D5:D5">
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="D5:D6">
       <x:formula1>4</x:formula1>
       <x:formula2/>
     </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="F5:F5">
-      <x:formula1>1</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="G5:G5">
-      <x:formula1>5</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="B6:B6">
-      <x:formula1>3</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="C6:C6">
-      <x:formula1>1</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="D6:D6">
-      <x:formula1>4</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="B7:B7">
-      <x:formula1>3</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="C7:C7">
-      <x:formula1>1</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="D7:D7">
-      <x:formula1>1</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="A11:A11">
-      <x:formula1>2</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="B11:B11">
-      <x:formula1>3</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="C11:C11">
-      <x:formula1>2</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="D11:D11">
-      <x:formula1>5</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="E11:E11">
-      <x:formula1>2</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="A12:A12">
-      <x:formula1>2</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="B12:B12">
-      <x:formula1>3</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="C12:C12">
-      <x:formula1>2</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="D12:D12">
-      <x:formula1>5</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="E12:E12">
-      <x:formula1>2</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="A13:A13">
-      <x:formula1>2</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="B13:B13">
-      <x:formula1>2</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="C13:C13">
-      <x:formula1>5</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="D13:D13">
-      <x:formula1>2</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="E13:E13">
-      <x:formula1>2</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="A14:A14">
-      <x:formula1>2</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="B14:B14">
-      <x:formula1>2</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="C14:C14">
-      <x:formula1>5</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="D14:D14">
-      <x:formula1>2</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="E14:E14">
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="A11:A14 C11:C12 E11:E14 B13:B14 D13:D14">
       <x:formula1>2</x:formula1>
       <x:formula2/>
     </x:dataValidation>

</xml_diff>

<commit_message>
MergedRanges copying removed as it's performed with rows copying. Minor changes in reference file
</commit_message>
<xml_diff>
--- a/ClosedXML_Tests/Resource/Examples/Misc/DataValidation.xlsx
+++ b/ClosedXML_Tests/Resource/Examples/Misc/DataValidation.xlsx
@@ -532,12 +532,48 @@
       <x:c r="E14" s="1" t="s"/>
     </x:row>
   </x:sheetData>
-  <x:dataValidations count="5">
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="A1:B1 A2:A2 C4:D4 F4:F5 C5:C7 D7:D7">
-      <x:formula1>1</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="A11:A14 C11:C12 E11:E14 B13:B14 D13:D14">
+  <x:dataValidations count="16">
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="A1:A2">
+      <x:formula1>1</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="B1:B1">
+      <x:formula1>1</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="C4:C7">
+      <x:formula1>1</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="D4:D4">
+      <x:formula1>1</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="D7:D7">
+      <x:formula1>1</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="F4:F5">
+      <x:formula1>1</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="A11:A14">
+      <x:formula1>2</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="B13:B14">
+      <x:formula1>2</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="E11:E14">
+      <x:formula1>2</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="C11:C12">
+      <x:formula1>2</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="D13:D14">
       <x:formula1>2</x:formula1>
       <x:formula2/>
     </x:dataValidation>
@@ -549,7 +585,15 @@
       <x:formula1>4</x:formula1>
       <x:formula2/>
     </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="G4:G5 D11:D12 C13:C14">
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="C13:C14">
+      <x:formula1>5</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="D11:D12">
+      <x:formula1>5</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="G4:G5">
       <x:formula1>5</x:formula1>
       <x:formula2/>
     </x:dataValidation>
@@ -578,6 +622,7 @@
   <x:sheetData>
     <x:row r="1" spans="1:3">
       <x:c r="A1" s="0" t="s"/>
+      <x:c r="B1" s="0" t="s"/>
       <x:c r="C1" s="0" t="s">
         <x:v>0</x:v>
       </x:c>
@@ -717,12 +762,48 @@
       <x:c r="E14" s="1" t="s"/>
     </x:row>
   </x:sheetData>
-  <x:dataValidations count="5">
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="A1:B1 A2:A2 C4:D4 F4:F5 C5:C7 D7:D7">
-      <x:formula1>1</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="A11:A14 C11:C12 E11:E14 B13:B14 D13:D14">
+  <x:dataValidations count="16">
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="B1:B1">
+      <x:formula1>1</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="D4:D4">
+      <x:formula1>1</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="D7:D7">
+      <x:formula1>1</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="A1:A2">
+      <x:formula1>1</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="C4:C7">
+      <x:formula1>1</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="F4:F5">
+      <x:formula1>1</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="A11:A14">
+      <x:formula1>2</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="B13:B14">
+      <x:formula1>2</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="E11:E14">
+      <x:formula1>2</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="C11:C12">
+      <x:formula1>2</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="D13:D14">
       <x:formula1>2</x:formula1>
       <x:formula2/>
     </x:dataValidation>
@@ -734,7 +815,15 @@
       <x:formula1>4</x:formula1>
       <x:formula2/>
     </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="G4:G5 D11:D12 C13:C14">
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="C13:C14">
+      <x:formula1>5</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="D11:D12">
+      <x:formula1>5</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="G4:G5">
       <x:formula1>5</x:formula1>
       <x:formula2/>
     </x:dataValidation>
@@ -884,24 +973,164 @@
       <x:c r="E14" s="1" t="s"/>
     </x:row>
   </x:sheetData>
-  <x:dataValidations count="5">
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="A1:B1 A2:A2 C4:D4 F4:F5 C5:C7 D7:D7">
-      <x:formula1>1</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="B2:B12">
+  <x:dataValidations count="40">
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="A1:A1">
+      <x:formula1>1</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="B1:B1">
+      <x:formula1>1</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="A2:A2">
+      <x:formula1>1</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="B2:B2">
       <x:formula1>3</x:formula1>
       <x:formula2/>
     </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="G4:G5 D11:D12 C13:C14">
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="B4:B4">
+      <x:formula1>3</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="C4:C4">
+      <x:formula1>1</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="D4:D4">
+      <x:formula1>1</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="F4:F4">
+      <x:formula1>1</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="G4:G4">
       <x:formula1>5</x:formula1>
       <x:formula2/>
     </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="D5:D6">
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="B5:B5">
+      <x:formula1>3</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="C5:C5">
+      <x:formula1>1</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="D5:D5">
       <x:formula1>4</x:formula1>
       <x:formula2/>
     </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="A11:A14 C11:C12 E11:E14 B13:B14 D13:D14">
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="F5:F5">
+      <x:formula1>1</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="G5:G5">
+      <x:formula1>5</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="B6:B6">
+      <x:formula1>3</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="C6:C6">
+      <x:formula1>1</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="D6:D6">
+      <x:formula1>4</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="B7:B7">
+      <x:formula1>3</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="C7:C7">
+      <x:formula1>1</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="D7:D7">
+      <x:formula1>1</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="A11:A11">
+      <x:formula1>2</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="B11:B11">
+      <x:formula1>3</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="C11:C11">
+      <x:formula1>2</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="D11:D11">
+      <x:formula1>5</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="E11:E11">
+      <x:formula1>2</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="A12:A12">
+      <x:formula1>2</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="B12:B12">
+      <x:formula1>3</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="C12:C12">
+      <x:formula1>2</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="D12:D12">
+      <x:formula1>5</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="E12:E12">
+      <x:formula1>2</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="A13:A13">
+      <x:formula1>2</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="B13:B13">
+      <x:formula1>2</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="C13:C13">
+      <x:formula1>5</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="D13:D13">
+      <x:formula1>2</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="E13:E13">
+      <x:formula1>2</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="A14:A14">
+      <x:formula1>2</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="B14:B14">
+      <x:formula1>2</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="C14:C14">
+      <x:formula1>5</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="D14:D14">
+      <x:formula1>2</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="E14:E14">
       <x:formula1>2</x:formula1>
       <x:formula2/>
     </x:dataValidation>

</xml_diff>

<commit_message>
Сonsolidation of conditional formats and data validation rules (#761)
* Failing test added

* Multiple ranges for conditional format

* Clearing ranges of CF fixed.

* XLConditionalFormat.Range implemented via Ranges.

* Tests for CF copying added

* XLRangeConsolidationEngine implemented

* Conditional formats consolidation re-implemented.

* Data validaton rules consolidation implemented

* Tests fixed

* CF formula adjustment implemented

* Fix clearing formats not covered by cleared range

* Reference files updated (uncertain about changes). Adjusting CF formulas fixed

* Fix multi-range conditional formats loading. Fix CF consolidation to prevent reordering of rules.

* Fix formula shifting for multi-ranged conditional formats.

* Merge conflicts solved

* Range property made non-obsolete and returning First rather than Single
</commit_message>
<xml_diff>
--- a/ClosedXML_Tests/Resource/Examples/Misc/DataValidation.xlsx
+++ b/ClosedXML_Tests/Resource/Examples/Misc/DataValidation.xlsx
@@ -532,48 +532,12 @@
       <x:c r="E14" s="1" t="s"/>
     </x:row>
   </x:sheetData>
-  <x:dataValidations count="16">
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="A1:A2">
+  <x:dataValidations count="5">
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="A1:B1 A2:A2 C4:D4 F4:F5 C5:C7 D7:D7">
       <x:formula1>1</x:formula1>
       <x:formula2/>
     </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="B1:B1">
-      <x:formula1>1</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="C4:C7">
-      <x:formula1>1</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="D4:D4">
-      <x:formula1>1</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="D7:D7">
-      <x:formula1>1</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="F4:F5">
-      <x:formula1>1</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="A11:A14">
-      <x:formula1>2</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="B13:B14">
-      <x:formula1>2</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="E11:E14">
-      <x:formula1>2</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="C11:C12">
-      <x:formula1>2</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="D13:D14">
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="A11:A14 C11:C12 E11:E14 B13:B14 D13:D14">
       <x:formula1>2</x:formula1>
       <x:formula2/>
     </x:dataValidation>
@@ -585,15 +549,7 @@
       <x:formula1>4</x:formula1>
       <x:formula2/>
     </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="C13:C14">
-      <x:formula1>5</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="D11:D12">
-      <x:formula1>5</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="G4:G5">
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="G4:G5 D11:D12 C13:C14">
       <x:formula1>5</x:formula1>
       <x:formula2/>
     </x:dataValidation>
@@ -761,48 +717,12 @@
       <x:c r="E14" s="1" t="s"/>
     </x:row>
   </x:sheetData>
-  <x:dataValidations count="16">
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="A1:A2">
+  <x:dataValidations count="5">
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="A1:B1 A2:A2 C4:D4 F4:F5 C5:C7 D7:D7">
       <x:formula1>1</x:formula1>
       <x:formula2/>
     </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="B1:B1">
-      <x:formula1>1</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="C4:C7">
-      <x:formula1>1</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="D4:D4">
-      <x:formula1>1</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="D7:D7">
-      <x:formula1>1</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="F4:F5">
-      <x:formula1>1</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="A11:A14">
-      <x:formula1>2</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="B13:B14">
-      <x:formula1>2</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="E11:E14">
-      <x:formula1>2</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="C11:C12">
-      <x:formula1>2</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="D13:D14">
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="A11:A14 C11:C12 E11:E14 B13:B14 D13:D14">
       <x:formula1>2</x:formula1>
       <x:formula2/>
     </x:dataValidation>
@@ -814,15 +734,7 @@
       <x:formula1>4</x:formula1>
       <x:formula2/>
     </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="C13:C14">
-      <x:formula1>5</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="D11:D12">
-      <x:formula1>5</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="G4:G5">
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="G4:G5 D11:D12 C13:C14">
       <x:formula1>5</x:formula1>
       <x:formula2/>
     </x:dataValidation>
@@ -972,164 +884,24 @@
       <x:c r="E14" s="1" t="s"/>
     </x:row>
   </x:sheetData>
-  <x:dataValidations count="40">
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="A1:A1">
+  <x:dataValidations count="5">
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="A1:B1 A2:A2 C4:D4 F4:F5 C5:C7 D7:D7">
       <x:formula1>1</x:formula1>
       <x:formula2/>
     </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="B1:B1">
-      <x:formula1>1</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="A2:A2">
-      <x:formula1>1</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="B2:B2">
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="B2:B12">
       <x:formula1>3</x:formula1>
       <x:formula2/>
     </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="B4:B4">
-      <x:formula1>3</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="C4:C4">
-      <x:formula1>1</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="D4:D4">
-      <x:formula1>1</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="F4:F4">
-      <x:formula1>1</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="G4:G4">
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="G4:G5 D11:D12 C13:C14">
       <x:formula1>5</x:formula1>
       <x:formula2/>
     </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="B5:B5">
-      <x:formula1>3</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="C5:C5">
-      <x:formula1>1</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="D5:D5">
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="D5:D6">
       <x:formula1>4</x:formula1>
       <x:formula2/>
     </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="F5:F5">
-      <x:formula1>1</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="G5:G5">
-      <x:formula1>5</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="B6:B6">
-      <x:formula1>3</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="C6:C6">
-      <x:formula1>1</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="D6:D6">
-      <x:formula1>4</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="B7:B7">
-      <x:formula1>3</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="C7:C7">
-      <x:formula1>1</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="D7:D7">
-      <x:formula1>1</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="A11:A11">
-      <x:formula1>2</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="B11:B11">
-      <x:formula1>3</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="C11:C11">
-      <x:formula1>2</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="D11:D11">
-      <x:formula1>5</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="E11:E11">
-      <x:formula1>2</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="A12:A12">
-      <x:formula1>2</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="B12:B12">
-      <x:formula1>3</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="C12:C12">
-      <x:formula1>2</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="D12:D12">
-      <x:formula1>5</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="E12:E12">
-      <x:formula1>2</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="A13:A13">
-      <x:formula1>2</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="B13:B13">
-      <x:formula1>2</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="C13:C13">
-      <x:formula1>5</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="D13:D13">
-      <x:formula1>2</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="E13:E13">
-      <x:formula1>2</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="A14:A14">
-      <x:formula1>2</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="B14:B14">
-      <x:formula1>2</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="C14:C14">
-      <x:formula1>5</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="D14:D14">
-      <x:formula1>2</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="E14:E14">
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="A11:A14 C11:C12 E11:E14 B13:B14 D13:D14">
       <x:formula1>2</x:formula1>
       <x:formula2/>
     </x:dataValidation>

</xml_diff>

<commit_message>
Update XLCell.MergedRange to use GetIntersectedRanges
</commit_message>
<xml_diff>
--- a/ClosedXML_Tests/Resource/Examples/Misc/DataValidation.xlsx
+++ b/ClosedXML_Tests/Resource/Examples/Misc/DataValidation.xlsx
@@ -577,8 +577,6 @@
   </x:cols>
   <x:sheetData>
     <x:row r="1" spans="1:3">
-      <x:c r="A1" s="0" t="s"/>
-      <x:c r="B1" s="0" t="s"/>
       <x:c r="C1" s="0" t="s">
         <x:v>0</x:v>
       </x:c>
@@ -587,15 +585,6 @@
       <x:c r="C2" s="0" t="s">
         <x:v>1</x:v>
       </x:c>
-    </x:row>
-    <x:row r="4" spans="1:3">
-      <x:c r="A4" s="0" t="s"/>
-    </x:row>
-    <x:row r="5" spans="1:3">
-      <x:c r="A5" s="0" t="s"/>
-    </x:row>
-    <x:row r="6" spans="1:3">
-      <x:c r="A6" s="0" t="s"/>
     </x:row>
   </x:sheetData>
   <x:dataValidations count="7">

</xml_diff>

<commit_message>
Fix unit-test ordering issue
</commit_message>
<xml_diff>
--- a/ClosedXML_Tests/Resource/Examples/Misc/DataValidation.xlsx
+++ b/ClosedXML_Tests/Resource/Examples/Misc/DataValidation.xlsx
@@ -578,14 +578,6 @@
     </x:row>
   </x:sheetData>
   <x:dataValidations count="7">
-    <x:dataValidation type="whole" errorStyle="stop" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="B1:B2">
-      <x:formula1>1</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="whole" errorStyle="stop" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="B3:B4">
-      <x:formula1>2</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
     <x:dataValidation type="decimal" errorStyle="stop" operator="between" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="A1:A1">
       <x:formula1>1</x:formula1>
       <x:formula2>5</x:formula2>
@@ -604,6 +596,14 @@
     </x:dataValidation>
     <x:dataValidation type="list" errorStyle="stop" operator="between" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="A6:A6">
       <x:formula1>=YesNo</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="whole" errorStyle="stop" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="B1:B2">
+      <x:formula1>1</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="whole" errorStyle="stop" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="B3:B4">
+      <x:formula1>2</x:formula1>
       <x:formula2/>
     </x:dataValidation>
   </x:dataValidations>
@@ -702,12 +702,12 @@
       <x:formula1>1</x:formula1>
       <x:formula2/>
     </x:dataValidation>
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="A11:A14 C11:C12 E11:E14 B13:B14 D13:D14">
+      <x:formula1>2</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
     <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="B2:B12">
       <x:formula1>3</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="A11:A14 C11:C12 E11:E14 B13:B14 D13:D14">
-      <x:formula1>2</x:formula1>
       <x:formula2/>
     </x:dataValidation>
     <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="D5:D6">

</xml_diff>

<commit_message>
Update a reference file (order of data validation rules changed)
</commit_message>
<xml_diff>
--- a/ClosedXML_Tests/Resource/Examples/Misc/DataValidation.xlsx
+++ b/ClosedXML_Tests/Resource/Examples/Misc/DataValidation.xlsx
@@ -702,12 +702,12 @@
       <x:formula1>1</x:formula1>
       <x:formula2/>
     </x:dataValidation>
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="A11:A14 C11:C12 E11:E14 B13:B14 D13:D14">
+      <x:formula1>2</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
     <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="B2:B12">
       <x:formula1>3</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="A11:A14 C11:C12 E11:E14 B13:B14 D13:D14">
-      <x:formula1>2</x:formula1>
       <x:formula2/>
     </x:dataValidation>
     <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="D5:D6">
@@ -739,7 +739,7 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:C6"/>
+  <x:dimension ref="A1:C2"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
@@ -761,28 +761,28 @@
       <x:formula1>1</x:formula1>
       <x:formula2>5</x:formula2>
     </x:dataValidation>
+    <x:dataValidation type="whole" errorStyle="warning" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Number out of range" error="This cell only allows the number 2." promptTitle="" prompt="" sqref="A2:A3">
+      <x:formula1>2</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="date" errorStyle="stop" operator="greaterThanOrEqual" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="Can't party like it's 1999." prompt="Please enter a date in this century." sqref="A4:A4">
+      <x:formula1>36526</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="list" errorStyle="stop" operator="between" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="A5:A5">
+      <x:formula1>'Data Validation'!$C$1:$C$2</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="list" errorStyle="stop" operator="between" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="A6:A6">
+      <x:formula1>=YesNo</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
     <x:dataValidation type="whole" errorStyle="stop" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="B1:B2">
       <x:formula1>1</x:formula1>
       <x:formula2/>
     </x:dataValidation>
-    <x:dataValidation type="whole" errorStyle="warning" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Number out of range" error="This cell only allows the number 2." promptTitle="" prompt="" sqref="A2:A3">
-      <x:formula1>2</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
     <x:dataValidation type="whole" errorStyle="stop" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="B3:B4">
       <x:formula1>2</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="date" errorStyle="stop" operator="greaterThanOrEqual" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="Can't party like it's 1999." prompt="Please enter a date in this century." sqref="A4:A4">
-      <x:formula1>36526</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="list" errorStyle="stop" operator="between" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="A5:A5">
-      <x:formula1>'Data Validation'!$C$1:$C$2</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="list" errorStyle="stop" operator="between" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="A6:A6">
-      <x:formula1>=YesNo</x:formula1>
       <x:formula2/>
     </x:dataValidation>
   </x:dataValidations>
@@ -871,20 +871,20 @@
       <x:formula1>1</x:formula1>
       <x:formula2/>
     </x:dataValidation>
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="A11:A14 C11:C12 E11:E14 B13:B14 D13:D14">
+      <x:formula1>2</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
     <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="B2:B12">
       <x:formula1>3</x:formula1>
       <x:formula2/>
     </x:dataValidation>
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="D5:D6">
+      <x:formula1>4</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
     <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="G4:G5 D11:D12 C13:C14">
       <x:formula1>5</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="D5:D6">
-      <x:formula1>4</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="A11:A14 C11:C12 E11:E14 B13:B14 D13:D14">
-      <x:formula1>2</x:formula1>
       <x:formula2/>
     </x:dataValidation>
   </x:dataValidations>

</xml_diff>

<commit_message>
Update a reference file (the order of data validation rules has changed)
</commit_message>
<xml_diff>
--- a/ClosedXML_Tests/Resource/Examples/Misc/DataValidation.xlsx
+++ b/ClosedXML_Tests/Resource/Examples/Misc/DataValidation.xlsx
@@ -394,9 +394,6 @@
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15"/>
-  <x:cols>
-    <x:col min="1" max="2" width="9.140625" style="0" customWidth="1"/>
-  </x:cols>
   <x:sheetData>
     <x:row r="1" spans="1:3">
       <x:c r="C1" s="0" t="s">
@@ -457,9 +454,6 @@
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15"/>
-  <x:cols>
-    <x:col min="1" max="4" width="9.140625" style="0" customWidth="1"/>
-  </x:cols>
   <x:sheetData>
     <x:row r="1" spans="1:7">
       <x:c r="A1" s="1" t="s"/>
@@ -562,9 +556,6 @@
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15"/>
-  <x:cols>
-    <x:col min="1" max="2" width="9.140625" style="0" customWidth="1"/>
-  </x:cols>
   <x:sheetData>
     <x:row r="1" spans="1:3">
       <x:c r="C1" s="0" t="s">
@@ -578,14 +569,6 @@
     </x:row>
   </x:sheetData>
   <x:dataValidations count="7">
-    <x:dataValidation type="whole" errorStyle="stop" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="B1:B2">
-      <x:formula1>1</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="whole" errorStyle="stop" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="B3:B4">
-      <x:formula1>2</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
     <x:dataValidation type="decimal" errorStyle="stop" operator="between" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="A1:A1">
       <x:formula1>1</x:formula1>
       <x:formula2>5</x:formula2>
@@ -604,6 +587,14 @@
     </x:dataValidation>
     <x:dataValidation type="list" errorStyle="stop" operator="between" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="A6:A6">
       <x:formula1>=YesNo</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="whole" errorStyle="stop" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="B1:B2">
+      <x:formula1>1</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="whole" errorStyle="stop" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="B3:B4">
+      <x:formula1>2</x:formula1>
       <x:formula2/>
     </x:dataValidation>
   </x:dataValidations>
@@ -632,9 +623,6 @@
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15"/>
-  <x:cols>
-    <x:col min="1" max="4" width="9.140625" style="0" customWidth="1"/>
-  </x:cols>
   <x:sheetData>
     <x:row r="1" spans="1:7">
       <x:c r="A1" s="1" t="s"/>

</xml_diff>

<commit_message>
Fix subscription/unsubscription of data validation rules during the consolidation
</commit_message>
<xml_diff>
--- a/ClosedXML_Tests/Resource/Examples/Misc/DataValidation.xlsx
+++ b/ClosedXML_Tests/Resource/Examples/Misc/DataValidation.xlsx
@@ -859,20 +859,20 @@
       <x:formula1>1</x:formula1>
       <x:formula2/>
     </x:dataValidation>
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="B2:B12">
+      <x:formula1>3</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="G4:G5 D11:D12 C13:C14">
+      <x:formula1>5</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="D5:D6">
+      <x:formula1>4</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
     <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="A11:A14 C11:C12 E11:E14 B13:B14 D13:D14">
       <x:formula1>2</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="B2:B12">
-      <x:formula1>3</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="D5:D6">
-      <x:formula1>4</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="G4:G5 D11:D12 C13:C14">
-      <x:formula1>5</x:formula1>
       <x:formula2/>
     </x:dataValidation>
   </x:dataValidations>

</xml_diff>

<commit_message>
Increase code coverage in data validations. Make number conversion culture-independent
</commit_message>
<xml_diff>
--- a/ClosedXML_Tests/Resource/Examples/Misc/DataValidation.xlsx
+++ b/ClosedXML_Tests/Resource/Examples/Misc/DataValidation.xlsx
@@ -45,7 +45,7 @@
       <x:family val="2"/>
     </x:font>
   </x:fonts>
-  <x:fills count="3">
+  <x:fills count="10">
     <x:fill>
       <x:patternFill patternType="none"/>
     </x:fill>
@@ -55,6 +55,41 @@
     <x:fill>
       <x:patternFill patternType="solid">
         <x:fgColor rgb="FF9ACD32"/>
+      </x:patternFill>
+    </x:fill>
+    <x:fill>
+      <x:patternFill patternType="solid">
+        <x:fgColor rgb="FF00FFFF"/>
+      </x:patternFill>
+    </x:fill>
+    <x:fill>
+      <x:patternFill patternType="solid">
+        <x:fgColor rgb="FFEFDECD"/>
+      </x:patternFill>
+    </x:fill>
+    <x:fill>
+      <x:patternFill patternType="solid">
+        <x:fgColor rgb="FFFBCEB1"/>
+      </x:patternFill>
+    </x:fill>
+    <x:fill>
+      <x:patternFill patternType="solid">
+        <x:fgColor rgb="FFE52B50"/>
+      </x:patternFill>
+    </x:fill>
+    <x:fill>
+      <x:patternFill patternType="solid">
+        <x:fgColor rgb="FFE32636"/>
+      </x:patternFill>
+    </x:fill>
+    <x:fill>
+      <x:patternFill patternType="solid">
+        <x:fgColor rgb="FF9966CC"/>
+      </x:patternFill>
+    </x:fill>
+    <x:fill>
+      <x:patternFill patternType="solid">
+        <x:fgColor rgb="FFFFBF00"/>
       </x:patternFill>
     </x:fill>
   </x:fills>
@@ -77,20 +112,69 @@
       </x:diagonal>
     </x:border>
   </x:borders>
-  <x:cellStyleXfs count="2">
+  <x:cellStyleXfs count="9">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
     <x:xf numFmtId="0" fontId="0" fillId="2" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="3" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="4" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="5" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="6" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="7" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="8" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="9" borderId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
   </x:cellStyleXfs>
-  <x:cellXfs count="2">
+  <x:cellXfs count="9">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
     </x:xf>
     <x:xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
     </x:xf>
@@ -449,93 +533,129 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:G14"/>
+  <x:dimension ref="A1:H14"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15"/>
   <x:sheetData>
-    <x:row r="1" spans="1:7">
+    <x:row r="1" spans="1:8">
       <x:c r="A1" s="1" t="s"/>
       <x:c r="B1" s="1" t="s"/>
-    </x:row>
-    <x:row r="2" spans="1:7">
+      <x:c r="H1" s="2" t="s"/>
+    </x:row>
+    <x:row r="2" spans="1:8">
       <x:c r="A2" s="1" t="s"/>
-      <x:c r="B2" s="1" t="s"/>
-    </x:row>
-    <x:row r="4" spans="1:7">
-      <x:c r="B4" s="1" t="s"/>
+      <x:c r="B2" s="3" t="s"/>
+      <x:c r="H2" s="2" t="s"/>
+    </x:row>
+    <x:row r="3" spans="1:8">
+      <x:c r="B3" s="3" t="s"/>
+      <x:c r="H3" s="2" t="s"/>
+    </x:row>
+    <x:row r="4" spans="1:8">
+      <x:c r="B4" s="3" t="s"/>
       <x:c r="C4" s="1" t="s"/>
       <x:c r="D4" s="1" t="s"/>
       <x:c r="F4" s="1" t="s"/>
-      <x:c r="G4" s="1" t="s"/>
-    </x:row>
-    <x:row r="5" spans="1:7">
-      <x:c r="B5" s="1" t="s"/>
+      <x:c r="G4" s="4" t="s"/>
+      <x:c r="H4" s="2" t="s"/>
+    </x:row>
+    <x:row r="5" spans="1:8">
+      <x:c r="B5" s="3" t="s"/>
       <x:c r="C5" s="1" t="s"/>
-      <x:c r="D5" s="1" t="s"/>
+      <x:c r="D5" s="5" t="s"/>
       <x:c r="F5" s="1" t="s"/>
-      <x:c r="G5" s="1" t="s"/>
-    </x:row>
-    <x:row r="6" spans="1:7">
-      <x:c r="B6" s="1" t="s"/>
+      <x:c r="G5" s="4" t="s"/>
+      <x:c r="H5" s="2" t="s"/>
+    </x:row>
+    <x:row r="6" spans="1:8">
+      <x:c r="B6" s="3" t="s"/>
       <x:c r="C6" s="1" t="s"/>
-      <x:c r="D6" s="1" t="s"/>
-    </x:row>
-    <x:row r="7" spans="1:7">
-      <x:c r="B7" s="1" t="s"/>
+      <x:c r="D6" s="5" t="s"/>
+      <x:c r="H6" s="2" t="s"/>
+    </x:row>
+    <x:row r="7" spans="1:8">
+      <x:c r="B7" s="3" t="s"/>
       <x:c r="C7" s="1" t="s"/>
       <x:c r="D7" s="1" t="s"/>
-    </x:row>
-    <x:row r="11" spans="1:7">
-      <x:c r="A11" s="1" t="s"/>
-      <x:c r="B11" s="1" t="s"/>
-      <x:c r="C11" s="1" t="s"/>
-      <x:c r="D11" s="1" t="s"/>
-      <x:c r="E11" s="1" t="s"/>
-    </x:row>
-    <x:row r="12" spans="1:7">
-      <x:c r="A12" s="1" t="s"/>
-      <x:c r="B12" s="1" t="s"/>
-      <x:c r="C12" s="1" t="s"/>
-      <x:c r="D12" s="1" t="s"/>
-      <x:c r="E12" s="1" t="s"/>
-    </x:row>
-    <x:row r="13" spans="1:7">
-      <x:c r="A13" s="1" t="s"/>
-      <x:c r="B13" s="1" t="s"/>
-      <x:c r="C13" s="1" t="s"/>
-      <x:c r="D13" s="1" t="s"/>
-      <x:c r="E13" s="1" t="s"/>
-    </x:row>
-    <x:row r="14" spans="1:7">
-      <x:c r="A14" s="1" t="s"/>
-      <x:c r="B14" s="1" t="s"/>
-      <x:c r="C14" s="1" t="s"/>
-      <x:c r="D14" s="1" t="s"/>
-      <x:c r="E14" s="1" t="s"/>
+      <x:c r="H7" s="2" t="s"/>
+    </x:row>
+    <x:row r="8" spans="1:8">
+      <x:c r="B8" s="3" t="s"/>
+      <x:c r="H8" s="2" t="s"/>
+    </x:row>
+    <x:row r="9" spans="1:8">
+      <x:c r="B9" s="3" t="s"/>
+      <x:c r="H9" s="2" t="s"/>
+    </x:row>
+    <x:row r="10" spans="1:8">
+      <x:c r="B10" s="3" t="s"/>
+      <x:c r="H10" s="2" t="s"/>
+    </x:row>
+    <x:row r="11" spans="1:8">
+      <x:c r="A11" s="6" t="s"/>
+      <x:c r="B11" s="3" t="s"/>
+      <x:c r="C11" s="6" t="s"/>
+      <x:c r="D11" s="7" t="s"/>
+      <x:c r="E11" s="6" t="s"/>
+      <x:c r="H11" s="2" t="s"/>
+    </x:row>
+    <x:row r="12" spans="1:8">
+      <x:c r="A12" s="6" t="s"/>
+      <x:c r="B12" s="3" t="s"/>
+      <x:c r="C12" s="6" t="s"/>
+      <x:c r="D12" s="7" t="s"/>
+      <x:c r="E12" s="6" t="s"/>
+      <x:c r="H12" s="2" t="s"/>
+    </x:row>
+    <x:row r="13" spans="1:8">
+      <x:c r="A13" s="6" t="s"/>
+      <x:c r="B13" s="6" t="s"/>
+      <x:c r="C13" s="8" t="s"/>
+      <x:c r="D13" s="6" t="s"/>
+      <x:c r="E13" s="6" t="s"/>
+    </x:row>
+    <x:row r="14" spans="1:8">
+      <x:c r="A14" s="6" t="s"/>
+      <x:c r="B14" s="6" t="s"/>
+      <x:c r="C14" s="8" t="s"/>
+      <x:c r="D14" s="6" t="s"/>
+      <x:c r="E14" s="6" t="s"/>
     </x:row>
   </x:sheetData>
-  <x:dataValidations count="5">
+  <x:dataValidations count="8">
     <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="A1:B1 A2:A2 C4:D4 F4:F5 C5:C7 D7:D7">
-      <x:formula1>1</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="A11:A14 C11:C12 E11:E14 B13:B14 D13:D14">
-      <x:formula1>2</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="B2:B12">
-      <x:formula1>3</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="D5:D6">
-      <x:formula1>4</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="G4:G5 D11:D12 C13:C14">
-      <x:formula1>5</x:formula1>
-      <x:formula2/>
+      <x:formula1>1.1</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="decimal" errorStyle="stop" operator="notEqual" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="A11:A14 C11:C12 E11:E14 B13:B14 D13:D14">
+      <x:formula1>2.2</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="decimal" errorStyle="stop" operator="greaterThan" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="B2:B12">
+      <x:formula1>3.3</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="decimal" errorStyle="stop" operator="lessThan" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="D5:D6">
+      <x:formula1>4.4</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="decimal" errorStyle="stop" operator="greaterThanOrEqual" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="C13:C14">
+      <x:formula1>5.5</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="decimal" errorStyle="stop" operator="lessThanOrEqual" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="D11:D12">
+      <x:formula1>6.6</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="decimal" errorStyle="stop" operator="between" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="G4:G5">
+      <x:formula1>7.7</x:formula1>
+      <x:formula2>8.8</x:formula2>
+    </x:dataValidation>
+    <x:dataValidation type="decimal" errorStyle="stop" operator="notBetween" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="H1:H12">
+      <x:formula1>9.9</x:formula1>
+      <x:formula2>10.1</x:formula2>
     </x:dataValidation>
   </x:dataValidations>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
@@ -618,93 +738,129 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:G14"/>
+  <x:dimension ref="A1:H14"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15"/>
   <x:sheetData>
-    <x:row r="1" spans="1:7">
+    <x:row r="1" spans="1:8">
       <x:c r="A1" s="1" t="s"/>
       <x:c r="B1" s="1" t="s"/>
-    </x:row>
-    <x:row r="2" spans="1:7">
+      <x:c r="H1" s="2" t="s"/>
+    </x:row>
+    <x:row r="2" spans="1:8">
       <x:c r="A2" s="1" t="s"/>
-      <x:c r="B2" s="1" t="s"/>
-    </x:row>
-    <x:row r="4" spans="1:7">
-      <x:c r="B4" s="1" t="s"/>
+      <x:c r="B2" s="3" t="s"/>
+      <x:c r="H2" s="2" t="s"/>
+    </x:row>
+    <x:row r="3" spans="1:8">
+      <x:c r="B3" s="3" t="s"/>
+      <x:c r="H3" s="2" t="s"/>
+    </x:row>
+    <x:row r="4" spans="1:8">
+      <x:c r="B4" s="3" t="s"/>
       <x:c r="C4" s="1" t="s"/>
       <x:c r="D4" s="1" t="s"/>
       <x:c r="F4" s="1" t="s"/>
-      <x:c r="G4" s="1" t="s"/>
-    </x:row>
-    <x:row r="5" spans="1:7">
-      <x:c r="B5" s="1" t="s"/>
+      <x:c r="G4" s="4" t="s"/>
+      <x:c r="H4" s="2" t="s"/>
+    </x:row>
+    <x:row r="5" spans="1:8">
+      <x:c r="B5" s="3" t="s"/>
       <x:c r="C5" s="1" t="s"/>
-      <x:c r="D5" s="1" t="s"/>
+      <x:c r="D5" s="5" t="s"/>
       <x:c r="F5" s="1" t="s"/>
-      <x:c r="G5" s="1" t="s"/>
-    </x:row>
-    <x:row r="6" spans="1:7">
-      <x:c r="B6" s="1" t="s"/>
+      <x:c r="G5" s="4" t="s"/>
+      <x:c r="H5" s="2" t="s"/>
+    </x:row>
+    <x:row r="6" spans="1:8">
+      <x:c r="B6" s="3" t="s"/>
       <x:c r="C6" s="1" t="s"/>
-      <x:c r="D6" s="1" t="s"/>
-    </x:row>
-    <x:row r="7" spans="1:7">
-      <x:c r="B7" s="1" t="s"/>
+      <x:c r="D6" s="5" t="s"/>
+      <x:c r="H6" s="2" t="s"/>
+    </x:row>
+    <x:row r="7" spans="1:8">
+      <x:c r="B7" s="3" t="s"/>
       <x:c r="C7" s="1" t="s"/>
       <x:c r="D7" s="1" t="s"/>
-    </x:row>
-    <x:row r="11" spans="1:7">
-      <x:c r="A11" s="1" t="s"/>
-      <x:c r="B11" s="1" t="s"/>
-      <x:c r="C11" s="1" t="s"/>
-      <x:c r="D11" s="1" t="s"/>
-      <x:c r="E11" s="1" t="s"/>
-    </x:row>
-    <x:row r="12" spans="1:7">
-      <x:c r="A12" s="1" t="s"/>
-      <x:c r="B12" s="1" t="s"/>
-      <x:c r="C12" s="1" t="s"/>
-      <x:c r="D12" s="1" t="s"/>
-      <x:c r="E12" s="1" t="s"/>
-    </x:row>
-    <x:row r="13" spans="1:7">
-      <x:c r="A13" s="1" t="s"/>
-      <x:c r="B13" s="1" t="s"/>
-      <x:c r="C13" s="1" t="s"/>
-      <x:c r="D13" s="1" t="s"/>
-      <x:c r="E13" s="1" t="s"/>
-    </x:row>
-    <x:row r="14" spans="1:7">
-      <x:c r="A14" s="1" t="s"/>
-      <x:c r="B14" s="1" t="s"/>
-      <x:c r="C14" s="1" t="s"/>
-      <x:c r="D14" s="1" t="s"/>
-      <x:c r="E14" s="1" t="s"/>
+      <x:c r="H7" s="2" t="s"/>
+    </x:row>
+    <x:row r="8" spans="1:8">
+      <x:c r="B8" s="3" t="s"/>
+      <x:c r="H8" s="2" t="s"/>
+    </x:row>
+    <x:row r="9" spans="1:8">
+      <x:c r="B9" s="3" t="s"/>
+      <x:c r="H9" s="2" t="s"/>
+    </x:row>
+    <x:row r="10" spans="1:8">
+      <x:c r="B10" s="3" t="s"/>
+      <x:c r="H10" s="2" t="s"/>
+    </x:row>
+    <x:row r="11" spans="1:8">
+      <x:c r="A11" s="6" t="s"/>
+      <x:c r="B11" s="3" t="s"/>
+      <x:c r="C11" s="6" t="s"/>
+      <x:c r="D11" s="7" t="s"/>
+      <x:c r="E11" s="6" t="s"/>
+      <x:c r="H11" s="2" t="s"/>
+    </x:row>
+    <x:row r="12" spans="1:8">
+      <x:c r="A12" s="6" t="s"/>
+      <x:c r="B12" s="3" t="s"/>
+      <x:c r="C12" s="6" t="s"/>
+      <x:c r="D12" s="7" t="s"/>
+      <x:c r="E12" s="6" t="s"/>
+      <x:c r="H12" s="2" t="s"/>
+    </x:row>
+    <x:row r="13" spans="1:8">
+      <x:c r="A13" s="6" t="s"/>
+      <x:c r="B13" s="6" t="s"/>
+      <x:c r="C13" s="8" t="s"/>
+      <x:c r="D13" s="6" t="s"/>
+      <x:c r="E13" s="6" t="s"/>
+    </x:row>
+    <x:row r="14" spans="1:8">
+      <x:c r="A14" s="6" t="s"/>
+      <x:c r="B14" s="6" t="s"/>
+      <x:c r="C14" s="8" t="s"/>
+      <x:c r="D14" s="6" t="s"/>
+      <x:c r="E14" s="6" t="s"/>
     </x:row>
   </x:sheetData>
-  <x:dataValidations count="5">
+  <x:dataValidations count="8">
     <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="A1:B1 A2:A2 C4:D4 F4:F5 C5:C7 D7:D7">
-      <x:formula1>1</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="A11:A14 C11:C12 E11:E14 B13:B14 D13:D14">
-      <x:formula1>2</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="B2:B12">
-      <x:formula1>3</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="D5:D6">
-      <x:formula1>4</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="G4:G5 D11:D12 C13:C14">
-      <x:formula1>5</x:formula1>
-      <x:formula2/>
+      <x:formula1>1.1</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="decimal" errorStyle="stop" operator="notEqual" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="A11:A14 C11:C12 E11:E14 B13:B14 D13:D14">
+      <x:formula1>2.2</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="decimal" errorStyle="stop" operator="greaterThan" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="B2:B12">
+      <x:formula1>3.3</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="decimal" errorStyle="stop" operator="lessThan" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="D5:D6">
+      <x:formula1>4.4</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="decimal" errorStyle="stop" operator="greaterThanOrEqual" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="C13:C14">
+      <x:formula1>5.5</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="decimal" errorStyle="stop" operator="lessThanOrEqual" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="D11:D12">
+      <x:formula1>6.6</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="decimal" errorStyle="stop" operator="between" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="G4:G5">
+      <x:formula1>7.7</x:formula1>
+      <x:formula2>8.8</x:formula2>
+    </x:dataValidation>
+    <x:dataValidation type="decimal" errorStyle="stop" operator="notBetween" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="H1:H12">
+      <x:formula1>9.9</x:formula1>
+      <x:formula2>10.1</x:formula2>
     </x:dataValidation>
   </x:dataValidations>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
@@ -787,92 +943,128 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:G14"/>
+  <x:dimension ref="A1:H14"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15"/>
   <x:sheetData>
-    <x:row r="1" spans="1:7">
+    <x:row r="1" spans="1:8">
       <x:c r="A1" s="1" t="s"/>
       <x:c r="B1" s="1" t="s"/>
-    </x:row>
-    <x:row r="2" spans="1:7">
+      <x:c r="H1" s="2" t="s"/>
+    </x:row>
+    <x:row r="2" spans="1:8">
       <x:c r="A2" s="1" t="s"/>
-      <x:c r="B2" s="1" t="s"/>
-    </x:row>
-    <x:row r="4" spans="1:7">
-      <x:c r="B4" s="1" t="s"/>
+      <x:c r="B2" s="3" t="s"/>
+      <x:c r="H2" s="2" t="s"/>
+    </x:row>
+    <x:row r="3" spans="1:8">
+      <x:c r="B3" s="3" t="s"/>
+      <x:c r="H3" s="2" t="s"/>
+    </x:row>
+    <x:row r="4" spans="1:8">
+      <x:c r="B4" s="3" t="s"/>
       <x:c r="C4" s="1" t="s"/>
       <x:c r="D4" s="1" t="s"/>
       <x:c r="F4" s="1" t="s"/>
-      <x:c r="G4" s="1" t="s"/>
-    </x:row>
-    <x:row r="5" spans="1:7">
-      <x:c r="B5" s="1" t="s"/>
+      <x:c r="G4" s="4" t="s"/>
+      <x:c r="H4" s="2" t="s"/>
+    </x:row>
+    <x:row r="5" spans="1:8">
+      <x:c r="B5" s="3" t="s"/>
       <x:c r="C5" s="1" t="s"/>
-      <x:c r="D5" s="1" t="s"/>
+      <x:c r="D5" s="5" t="s"/>
       <x:c r="F5" s="1" t="s"/>
-      <x:c r="G5" s="1" t="s"/>
-    </x:row>
-    <x:row r="6" spans="1:7">
-      <x:c r="B6" s="1" t="s"/>
+      <x:c r="G5" s="4" t="s"/>
+      <x:c r="H5" s="2" t="s"/>
+    </x:row>
+    <x:row r="6" spans="1:8">
+      <x:c r="B6" s="3" t="s"/>
       <x:c r="C6" s="1" t="s"/>
-      <x:c r="D6" s="1" t="s"/>
-    </x:row>
-    <x:row r="7" spans="1:7">
-      <x:c r="B7" s="1" t="s"/>
+      <x:c r="D6" s="5" t="s"/>
+      <x:c r="H6" s="2" t="s"/>
+    </x:row>
+    <x:row r="7" spans="1:8">
+      <x:c r="B7" s="3" t="s"/>
       <x:c r="C7" s="1" t="s"/>
       <x:c r="D7" s="1" t="s"/>
-    </x:row>
-    <x:row r="11" spans="1:7">
-      <x:c r="A11" s="1" t="s"/>
-      <x:c r="B11" s="1" t="s"/>
-      <x:c r="C11" s="1" t="s"/>
-      <x:c r="D11" s="1" t="s"/>
-      <x:c r="E11" s="1" t="s"/>
-    </x:row>
-    <x:row r="12" spans="1:7">
-      <x:c r="A12" s="1" t="s"/>
-      <x:c r="B12" s="1" t="s"/>
-      <x:c r="C12" s="1" t="s"/>
-      <x:c r="D12" s="1" t="s"/>
-      <x:c r="E12" s="1" t="s"/>
-    </x:row>
-    <x:row r="13" spans="1:7">
-      <x:c r="A13" s="1" t="s"/>
-      <x:c r="B13" s="1" t="s"/>
-      <x:c r="C13" s="1" t="s"/>
-      <x:c r="D13" s="1" t="s"/>
-      <x:c r="E13" s="1" t="s"/>
-    </x:row>
-    <x:row r="14" spans="1:7">
-      <x:c r="A14" s="1" t="s"/>
-      <x:c r="B14" s="1" t="s"/>
-      <x:c r="C14" s="1" t="s"/>
-      <x:c r="D14" s="1" t="s"/>
-      <x:c r="E14" s="1" t="s"/>
+      <x:c r="H7" s="2" t="s"/>
+    </x:row>
+    <x:row r="8" spans="1:8">
+      <x:c r="B8" s="3" t="s"/>
+      <x:c r="H8" s="2" t="s"/>
+    </x:row>
+    <x:row r="9" spans="1:8">
+      <x:c r="B9" s="3" t="s"/>
+      <x:c r="H9" s="2" t="s"/>
+    </x:row>
+    <x:row r="10" spans="1:8">
+      <x:c r="B10" s="3" t="s"/>
+      <x:c r="H10" s="2" t="s"/>
+    </x:row>
+    <x:row r="11" spans="1:8">
+      <x:c r="A11" s="6" t="s"/>
+      <x:c r="B11" s="3" t="s"/>
+      <x:c r="C11" s="6" t="s"/>
+      <x:c r="D11" s="7" t="s"/>
+      <x:c r="E11" s="6" t="s"/>
+      <x:c r="H11" s="2" t="s"/>
+    </x:row>
+    <x:row r="12" spans="1:8">
+      <x:c r="A12" s="6" t="s"/>
+      <x:c r="B12" s="3" t="s"/>
+      <x:c r="C12" s="6" t="s"/>
+      <x:c r="D12" s="7" t="s"/>
+      <x:c r="E12" s="6" t="s"/>
+      <x:c r="H12" s="2" t="s"/>
+    </x:row>
+    <x:row r="13" spans="1:8">
+      <x:c r="A13" s="6" t="s"/>
+      <x:c r="B13" s="6" t="s"/>
+      <x:c r="C13" s="8" t="s"/>
+      <x:c r="D13" s="6" t="s"/>
+      <x:c r="E13" s="6" t="s"/>
+    </x:row>
+    <x:row r="14" spans="1:8">
+      <x:c r="A14" s="6" t="s"/>
+      <x:c r="B14" s="6" t="s"/>
+      <x:c r="C14" s="8" t="s"/>
+      <x:c r="D14" s="6" t="s"/>
+      <x:c r="E14" s="6" t="s"/>
     </x:row>
   </x:sheetData>
-  <x:dataValidations count="5">
+  <x:dataValidations count="8">
     <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="A1:B1 A2:A2 C4:D4 F4:F5 C5:C7 D7:D7">
-      <x:formula1>1</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="B2:B12">
-      <x:formula1>3</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="G4:G5 D11:D12 C13:C14">
-      <x:formula1>5</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="D5:D6">
-      <x:formula1>4</x:formula1>
-      <x:formula2/>
-    </x:dataValidation>
-    <x:dataValidation type="decimal" errorStyle="stop" operator="equal" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="A11:A14 C11:C12 E11:E14 B13:B14 D13:D14">
-      <x:formula1>2</x:formula1>
+      <x:formula1>1.1</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="decimal" errorStyle="stop" operator="notBetween" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="H1:H12">
+      <x:formula1>9.9</x:formula1>
+      <x:formula2>10.1</x:formula2>
+    </x:dataValidation>
+    <x:dataValidation type="decimal" errorStyle="stop" operator="greaterThan" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="B2:B12">
+      <x:formula1>3.3</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="decimal" errorStyle="stop" operator="between" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="G4:G5">
+      <x:formula1>7.7</x:formula1>
+      <x:formula2>8.8</x:formula2>
+    </x:dataValidation>
+    <x:dataValidation type="decimal" errorStyle="stop" operator="lessThan" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="D5:D6">
+      <x:formula1>4.4</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="decimal" errorStyle="stop" operator="notEqual" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="A11:A14 C11:C12 E11:E14 B13:B14 D13:D14">
+      <x:formula1>2.2</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="decimal" errorStyle="stop" operator="lessThanOrEqual" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="D11:D12">
+      <x:formula1>6.6</x:formula1>
+      <x:formula2/>
+    </x:dataValidation>
+    <x:dataValidation type="decimal" errorStyle="stop" operator="greaterThanOrEqual" allowBlank="1" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="" error="" promptTitle="" prompt="" sqref="C13:C14">
+      <x:formula1>5.5</x:formula1>
       <x:formula2/>
     </x:dataValidation>
   </x:dataValidations>

</xml_diff>